<commit_message>
Corrección de solicitud gráfica
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/SolicitudGrafica_CN_08_07_CO_REC200 ajustado.xlsx
+++ b/fuentes/contenidos/grado08/guion07/SolicitudGrafica_CN_08_07_CO_REC200 ajustado.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="205">
   <si>
     <t>Fecha:</t>
   </si>
@@ -390,9 +390,6 @@
     <t>Área:</t>
   </si>
   <si>
-    <t>CN_08_01_REC10</t>
-  </si>
-  <si>
     <t>CN_08_02_REC10_IMG01</t>
   </si>
   <si>
@@ -597,9 +594,6 @@
     <t>Fotografía</t>
   </si>
   <si>
-    <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/f/fc/Chronic_Myeloid_Leukemia_smear_2009-04-09.JPG </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://upload.wikimedia.org/wikipedia/commons/6/6e/Hutchinson-Gilford_Progeria_Syndrome.png </t>
   </si>
   <si>
@@ -630,9 +624,6 @@
     <t>Ilustrar la imagen. Traducir el título; queda “Síndrome de Turner”.</t>
   </si>
   <si>
-    <t>Niña con retraso mental</t>
-  </si>
-  <si>
     <t>Niño con la enfermedad de Canavan</t>
   </si>
   <si>
@@ -640,6 +631,12 @@
   </si>
   <si>
     <t>Hombre con extremidades anormalmente largas</t>
+  </si>
+  <si>
+    <t>Mujer con bebé</t>
+  </si>
+  <si>
+    <t>CN_08_07_CO_REC200</t>
   </si>
 </sst>
 </file>
@@ -2417,9 +2414,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="140" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2477,7 +2474,7 @@
       <c r="I2" s="58"/>
       <c r="J2" s="14"/>
       <c r="L2" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="M2" s="2" t="str">
         <f ca="1">IF($N2&lt;COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1+$N2,1,1,1),"")</f>
@@ -2508,7 +2505,7 @@
       <c r="I3" s="38"/>
       <c r="J3" s="14"/>
       <c r="L3" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M3" s="2" t="str">
         <f ca="1">IF($N3&lt;COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1+$N3,1,1,1),"")</f>
@@ -2528,7 +2525,7 @@
         <v>54</v>
       </c>
       <c r="C4" s="87" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D4" s="88"/>
       <c r="E4" s="5"/>
@@ -2560,7 +2557,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D5" s="90"/>
       <c r="E5" s="5"/>
@@ -2569,7 +2566,7 @@
         <v>Motor del recurso</v>
       </c>
       <c r="G5" s="61" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H5" s="58"/>
       <c r="I5" s="58"/>
@@ -2617,7 +2614,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>122</v>
+        <v>204</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>39</v>
@@ -2720,14 +2717,14 @@
         <v>Recurso F6</v>
       </c>
       <c r="D10" s="63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E10" s="63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F10" s="13" t="str">
         <f t="shared" ref="F10" ca="1" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_08_01_REC10_IMG01.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG01.jpg</v>
       </c>
       <c r="G10" s="13" t="str">
         <f ca="1">IF($F10&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2742,7 +2739,7 @@
         <v/>
       </c>
       <c r="J10" s="63" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K10" s="64"/>
       <c r="O10" s="2" t="str">
@@ -2755,22 +2752,22 @@
         <f t="shared" ref="A11:A18" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE(LEFT(A10,3),IF(MID(A10,4,2)+1&lt;10,CONCATENATE("0",MID(A10,4,2)+1))),"")</f>
         <v>IMG02</v>
       </c>
-      <c r="B11" s="62" t="s">
-        <v>191</v>
+      <c r="B11" s="62">
+        <v>98870129</v>
       </c>
       <c r="C11" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E11" s="63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F11" s="13" t="str">
         <f t="shared" ref="F11:F74" ca="1" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>CN_08_01_REC10_IMG02.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG02.jpg</v>
       </c>
       <c r="G11" s="13" t="str">
         <f ca="1">IF($F11&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2785,37 +2782,35 @@
         <v/>
       </c>
       <c r="J11" s="64" t="s">
-        <v>197</v>
-      </c>
-      <c r="K11" s="65" t="s">
-        <v>198</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="K11" s="65"/>
       <c r="O11" s="2" t="str">
         <f>'Definición técnica de imagenes'!A13</f>
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
       </c>
-      <c r="B12" s="62" t="s">
-        <v>192</v>
+      <c r="B12" s="62">
+        <v>256079260</v>
       </c>
       <c r="C12" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E12" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F12" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CN_08_01_REC10_IMG03n.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG03n.jpg</v>
       </c>
       <c r="G12" s="13" t="str">
         <f ca="1">IF($F12&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2823,44 +2818,42 @@
       </c>
       <c r="H12" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_08_01_REC10_IMG03a.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG03a.jpg</v>
       </c>
       <c r="I12" s="13" t="str">
         <f ca="1">IF(OR($B12&lt;&gt;"",$J12&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J12" s="64" t="s">
-        <v>199</v>
-      </c>
-      <c r="K12" s="64" t="s">
-        <v>198</v>
-      </c>
+        <v>195</v>
+      </c>
+      <c r="K12" s="64"/>
       <c r="O12" s="2" t="str">
         <f>'Definición técnica de imagenes'!A18</f>
         <v>Diaporama F1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="11" customFormat="1" ht="27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="11" customFormat="1" ht="67.5" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG04</v>
       </c>
-      <c r="B13" s="62">
-        <v>114653824</v>
+      <c r="B13" s="62" t="s">
+        <v>190</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
       </c>
       <c r="D13" s="63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E13" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F13" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CN_08_01_REC10_IMG04n.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG04n.jpg</v>
       </c>
       <c r="G13" s="13" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2868,17 +2861,17 @@
       </c>
       <c r="H13" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_08_01_REC10_IMG04a.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG04a.jpg</v>
       </c>
       <c r="I13" s="13" t="str">
         <f ca="1">IF(OR($B13&lt;&gt;"",$J13&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J13" s="64" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="K13" s="64" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
@@ -2891,21 +2884,21 @@
         <v>IMG05</v>
       </c>
       <c r="B14" s="62">
-        <v>98870129</v>
+        <v>114653824</v>
       </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
       </c>
       <c r="D14" s="63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E14" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F14" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CN_08_01_REC10_IMG05n.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG05n.jpg</v>
       </c>
       <c r="G14" s="13" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2913,16 +2906,18 @@
       </c>
       <c r="H14" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_08_01_REC10_IMG05a.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG05a.jpg</v>
       </c>
       <c r="I14" s="13" t="str">
         <f ca="1">IF(OR($B14&lt;&gt;"",$J14&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J14" s="64" t="s">
-        <v>202</v>
-      </c>
-      <c r="K14" s="64"/>
+        <v>198</v>
+      </c>
+      <c r="K14" s="64" t="s">
+        <v>196</v>
+      </c>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
         <v>F6</v>
@@ -2934,21 +2929,21 @@
         <v>IMG06</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
       </c>
       <c r="D15" s="63" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E15" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F15" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CN_08_01_REC10_IMG06n.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG06n.jpg</v>
       </c>
       <c r="G15" s="13" t="str">
         <f ca="1">IF($F15&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2956,16 +2951,18 @@
       </c>
       <c r="H15" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_08_01_REC10_IMG06a.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG06a.jpg</v>
       </c>
       <c r="I15" s="13" t="str">
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
-      <c r="J15" s="66" t="s">
-        <v>203</v>
-      </c>
-      <c r="K15" s="66"/>
+      <c r="J15" s="64" t="s">
+        <v>200</v>
+      </c>
+      <c r="K15" s="64" t="s">
+        <v>196</v>
+      </c>
       <c r="O15" s="2" t="str">
         <f>'Definición técnica de imagenes'!A24</f>
         <v>F6B</v>
@@ -2984,14 +2981,14 @@
         <v>Recurso F6</v>
       </c>
       <c r="D16" s="63" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E16" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F16" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CN_08_01_REC10_IMG07n.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG07n.jpg</v>
       </c>
       <c r="G16" s="13" t="str">
         <f ca="1">IF($F16&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -2999,14 +2996,14 @@
       </c>
       <c r="H16" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_08_01_REC10_IMG07a.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG07a.jpg</v>
       </c>
       <c r="I16" s="13" t="str">
         <f ca="1">IF(OR($B16&lt;&gt;"",$J16&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J16" s="67" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="K16" s="68"/>
       <c r="O16" s="2" t="str">
@@ -3020,21 +3017,21 @@
         <v>IMG08</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
         <v>Recurso F6</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E17" s="63" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F17" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>CN_08_01_REC10_IMG08n.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG08n.jpg</v>
       </c>
       <c r="G17" s="13" t="str">
         <f ca="1">IF($F17&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3042,16 +3039,18 @@
       </c>
       <c r="H17" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>CN_08_01_REC10_IMG08a.jpg</v>
+        <v>CN_08_07_CO_REC200_IMG08a.jpg</v>
       </c>
       <c r="I17" s="13" t="str">
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J17" s="66" t="s">
-        <v>205</v>
-      </c>
-      <c r="K17" s="66"/>
+        <v>202</v>
+      </c>
+      <c r="K17" s="66" t="s">
+        <v>196</v>
+      </c>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
         <v>F7B</v>
@@ -6711,7 +6710,7 @@
         <v>56</v>
       </c>
       <c r="B1" s="108" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C1" s="108" t="s">
         <v>63</v>
@@ -6753,7 +6752,7 @@
         <v>69</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C3" s="40" t="s">
         <v>70</v>
@@ -6769,7 +6768,7 @@
       </c>
       <c r="G3" s="40"/>
       <c r="H3" s="40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I3" s="40"/>
     </row>
@@ -6778,7 +6777,7 @@
         <v>57</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C4" s="42" t="s">
         <v>74</v>
@@ -6796,10 +6795,10 @@
         <v>76</v>
       </c>
       <c r="H4" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="42" t="s">
         <v>124</v>
-      </c>
-      <c r="I4" s="42" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6807,7 +6806,7 @@
         <v>77</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C5" s="42" t="s">
         <v>78</v>
@@ -6825,10 +6824,10 @@
         <v>76</v>
       </c>
       <c r="H5" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="42" t="s">
         <v>124</v>
-      </c>
-      <c r="I5" s="42" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6836,7 +6835,7 @@
         <v>58</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" s="42" t="s">
         <v>79</v>
@@ -6854,10 +6853,10 @@
         <v>76</v>
       </c>
       <c r="H6" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="42" t="s">
         <v>124</v>
-      </c>
-      <c r="I6" s="42" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="7" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6881,7 +6880,7 @@
       </c>
       <c r="G7" s="42"/>
       <c r="H7" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I7" s="42"/>
     </row>
@@ -6890,7 +6889,7 @@
         <v>80</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C8" s="42" t="s">
         <v>81</v>
@@ -6908,10 +6907,10 @@
         <v>76</v>
       </c>
       <c r="H8" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="42" t="s">
         <v>124</v>
-      </c>
-      <c r="I8" s="42" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6919,7 +6918,7 @@
         <v>82</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C9" s="42" t="s">
         <v>83</v>
@@ -6937,10 +6936,10 @@
         <v>76</v>
       </c>
       <c r="H9" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="42" t="s">
         <v>124</v>
-      </c>
-      <c r="I9" s="42" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6948,7 +6947,7 @@
         <v>84</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C10" s="42" t="s">
         <v>85</v>
@@ -6966,10 +6965,10 @@
         <v>76</v>
       </c>
       <c r="H10" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" s="42" t="s">
         <v>124</v>
-      </c>
-      <c r="I10" s="42" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -6977,7 +6976,7 @@
         <v>86</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C11" s="42" t="s">
         <v>87</v>
@@ -6993,7 +6992,7 @@
       </c>
       <c r="G11" s="42"/>
       <c r="H11" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I11" s="42"/>
     </row>
@@ -7002,7 +7001,7 @@
         <v>89</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C12" s="73" t="s">
         <v>90</v>
@@ -7020,10 +7019,10 @@
         <v>76</v>
       </c>
       <c r="H12" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" s="42" t="s">
         <v>124</v>
-      </c>
-      <c r="I12" s="42" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="41" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -7031,7 +7030,7 @@
         <v>91</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C13" s="42" t="s">
         <v>92</v>
@@ -7049,10 +7048,10 @@
         <v>76</v>
       </c>
       <c r="H13" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="42" t="s">
         <v>124</v>
-      </c>
-      <c r="I13" s="42" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -7075,7 +7074,7 @@
       </c>
       <c r="H14" s="42"/>
       <c r="I14" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="77" customFormat="1" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -7097,7 +7096,7 @@
       </c>
       <c r="G15" s="75"/>
       <c r="H15" s="76" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I15" s="75"/>
       <c r="J15" s="77" t="s">
@@ -7123,10 +7122,10 @@
         <v>116</v>
       </c>
       <c r="H16" s="46" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I16" s="46" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J16" s="47" t="s">
         <v>102</v>
@@ -7145,10 +7144,10 @@
         <v>72</v>
       </c>
       <c r="F17" s="42" t="s">
+        <v>156</v>
+      </c>
+      <c r="G17" s="42" t="s">
         <v>157</v>
-      </c>
-      <c r="G17" s="42" t="s">
-        <v>158</v>
       </c>
       <c r="H17" s="48" t="s">
         <v>104</v>
@@ -7162,13 +7161,13 @@
     </row>
     <row r="18" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B18" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D18" s="44" t="s">
         <v>71</v>
@@ -7181,17 +7180,17 @@
       </c>
       <c r="G18" s="44"/>
       <c r="H18" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I18" s="44"/>
       <c r="J18" s="49"/>
     </row>
     <row r="19" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B19" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C19" s="44"/>
       <c r="D19" s="44" t="s">
@@ -7201,21 +7200,21 @@
         <v>93</v>
       </c>
       <c r="F19" s="44" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G19" s="44"/>
       <c r="H19" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I19" s="44"/>
       <c r="J19" s="49"/>
     </row>
     <row r="20" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C20" s="44"/>
       <c r="D20" s="44" t="s">
@@ -7225,21 +7224,21 @@
         <v>93</v>
       </c>
       <c r="F20" s="44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G20" s="44"/>
       <c r="H20" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I20" s="44"/>
       <c r="J20" s="49"/>
     </row>
     <row r="21" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="42" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B21" s="42" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C21" s="44"/>
       <c r="D21" s="44" t="s">
@@ -7249,24 +7248,24 @@
         <v>93</v>
       </c>
       <c r="F21" s="44" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G21" s="44"/>
       <c r="H21" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I21" s="72"/>
       <c r="J21" s="49"/>
     </row>
     <row r="22" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="B22" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="C22" s="44" t="s">
         <v>133</v>
-      </c>
-      <c r="B22" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="C22" s="44" t="s">
-        <v>134</v>
       </c>
       <c r="D22" s="42" t="s">
         <v>71</v>
@@ -7275,22 +7274,22 @@
         <v>93</v>
       </c>
       <c r="F22" s="46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G22" s="44"/>
       <c r="H22" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
+        <v>132</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>155</v>
+      </c>
+      <c r="C23" s="44" t="s">
         <v>133</v>
-      </c>
-      <c r="B23" s="42" t="s">
-        <v>156</v>
-      </c>
-      <c r="C23" s="44" t="s">
-        <v>134</v>
       </c>
       <c r="D23" s="44" t="s">
         <v>71</v>
@@ -7299,24 +7298,24 @@
         <v>93</v>
       </c>
       <c r="F23" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="G23" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="G23" s="46" t="s">
-        <v>177</v>
-      </c>
       <c r="H23" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="44" t="s">
         <v>124</v>
-      </c>
-      <c r="I23" s="44" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="42" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C24" s="44"/>
       <c r="D24" s="44" t="s">
@@ -7326,23 +7325,23 @@
         <v>93</v>
       </c>
       <c r="F24" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="G24" s="46" t="s">
         <v>176</v>
-      </c>
-      <c r="G24" s="46" t="s">
-        <v>177</v>
       </c>
       <c r="H24" s="44"/>
       <c r="I24" s="72"/>
     </row>
     <row r="25" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" s="42" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D25" s="44" t="s">
         <v>71</v>
@@ -7351,22 +7350,22 @@
         <v>93</v>
       </c>
       <c r="F25" s="46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G25" s="46"/>
       <c r="H25" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B26" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C26" s="44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D26" s="44" t="s">
         <v>71</v>
@@ -7375,27 +7374,27 @@
         <v>93</v>
       </c>
       <c r="F26" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="G26" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="G26" s="46" t="s">
-        <v>177</v>
-      </c>
       <c r="H26" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" s="44" t="s">
         <v>124</v>
-      </c>
-      <c r="I26" s="44" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B27" s="42" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C27" s="44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D27" s="44" t="s">
         <v>71</v>
@@ -7404,22 +7403,22 @@
         <v>93</v>
       </c>
       <c r="F27" s="46" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G27" s="46"/>
       <c r="H27" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B28" s="42" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C28" s="44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D28" s="44" t="s">
         <v>71</v>
@@ -7428,22 +7427,22 @@
         <v>93</v>
       </c>
       <c r="F28" s="46" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G28" s="46"/>
       <c r="H28" s="42" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B29" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C29" s="44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D29" s="44" t="s">
         <v>71</v>
@@ -7452,27 +7451,27 @@
         <v>93</v>
       </c>
       <c r="F29" s="46" t="s">
+        <v>175</v>
+      </c>
+      <c r="G29" s="46" t="s">
         <v>176</v>
       </c>
-      <c r="G29" s="46" t="s">
-        <v>177</v>
-      </c>
       <c r="H29" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29" s="44" t="s">
         <v>124</v>
-      </c>
-      <c r="I29" s="44" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="42" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C30" s="44" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D30" s="44" t="s">
         <v>71</v>
@@ -7481,7 +7480,7 @@
         <v>93</v>
       </c>
       <c r="F30" s="44" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G30" s="44"/>
       <c r="H30" s="44"/>
@@ -7489,13 +7488,13 @@
     </row>
     <row r="31" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B31" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C31" s="44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D31" s="44"/>
       <c r="E31" s="44"/>
@@ -7506,10 +7505,10 @@
     </row>
     <row r="32" spans="1:10" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C32" s="44"/>
       <c r="D32" s="44"/>
@@ -7521,10 +7520,10 @@
     </row>
     <row r="33" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="42" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B33" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C33" s="44"/>
       <c r="D33" s="44" t="s">
@@ -7534,7 +7533,7 @@
         <v>93</v>
       </c>
       <c r="F33" s="44" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G33" s="44"/>
       <c r="H33" s="44"/>
@@ -7542,13 +7541,13 @@
     </row>
     <row r="34" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C34" s="44" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D34" s="44"/>
       <c r="E34" s="44"/>
@@ -7562,10 +7561,10 @@
         <v>95</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C35" s="44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D35" s="44" t="s">
         <v>71</v>
@@ -7574,16 +7573,16 @@
         <v>93</v>
       </c>
       <c r="F35" s="44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G35" s="44" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H35" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="I35" s="44" t="s">
         <v>124</v>
-      </c>
-      <c r="I35" s="44" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
@@ -7591,10 +7590,10 @@
         <v>95</v>
       </c>
       <c r="B36" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C36" s="44" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D36" s="44" t="s">
         <v>71</v>
@@ -7603,27 +7602,27 @@
         <v>93</v>
       </c>
       <c r="F36" s="44" t="s">
+        <v>180</v>
+      </c>
+      <c r="G36" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="G36" s="44" t="s">
-        <v>182</v>
-      </c>
       <c r="H36" s="44" t="s">
+        <v>123</v>
+      </c>
+      <c r="I36" s="44" t="s">
         <v>124</v>
-      </c>
-      <c r="I36" s="44" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D37" s="44" t="s">
         <v>71</v>
@@ -7632,7 +7631,7 @@
         <v>93</v>
       </c>
       <c r="F37" s="44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G37" s="44"/>
       <c r="H37" s="44"/>
@@ -7640,13 +7639,13 @@
     </row>
     <row r="38" spans="1:9" ht="14.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="42" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B38" s="42" t="s">
+        <v>169</v>
+      </c>
+      <c r="C38" s="44" t="s">
         <v>170</v>
-      </c>
-      <c r="C38" s="44" t="s">
-        <v>171</v>
       </c>
       <c r="D38" s="44" t="s">
         <v>71</v>
@@ -7655,7 +7654,7 @@
         <v>93</v>
       </c>
       <c r="F38" s="44" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G38" s="44"/>
       <c r="H38" s="44"/>
@@ -7673,7 +7672,7 @@
       </c>
       <c r="B41" s="51"/>
       <c r="C41" s="52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D41" s="53" t="s">
         <v>22</v>
@@ -7687,10 +7686,10 @@
       </c>
       <c r="B42" s="54"/>
       <c r="C42" s="60" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D42" s="56" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E42" s="55"/>
       <c r="F42" s="55"/>
@@ -7701,10 +7700,10 @@
       </c>
       <c r="B43" s="54"/>
       <c r="C43" s="60" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="56" t="s">
         <v>128</v>
-      </c>
-      <c r="D43" s="56" t="s">
-        <v>129</v>
       </c>
       <c r="E43" s="55"/>
       <c r="F43" s="55"/>
@@ -7715,10 +7714,10 @@
       </c>
       <c r="B44" s="54"/>
       <c r="C44" s="55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D44" s="56" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E44" s="55"/>
       <c r="F44" s="55"/>
@@ -7729,21 +7728,21 @@
       </c>
       <c r="B45" s="54"/>
       <c r="C45" s="55" t="s">
+        <v>130</v>
+      </c>
+      <c r="D45" s="56" t="s">
         <v>131</v>
-      </c>
-      <c r="D45" s="56" t="s">
-        <v>132</v>
       </c>
       <c r="E45" s="55"/>
       <c r="F45" s="55"/>
     </row>
     <row r="46" spans="1:9" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A46" s="54" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B46" s="54"/>
       <c r="C46" s="55" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D46" s="56" t="s">
         <v>113</v>

</xml_diff>